<commit_message>
chore: update Output.xlsx with latest data revisions
</commit_message>
<xml_diff>
--- a/Excel File Generator/Output.xlsx
+++ b/Excel File Generator/Output.xlsx
@@ -11,54 +11,177 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Account Number</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="56">
+  <si>
+    <t>Mandate Reference ID</t>
+  </si>
+  <si>
+    <t>Debit Account Name</t>
+  </si>
+  <si>
+    <t>Debit Account Number</t>
   </si>
   <si>
     <t>Routing Number</t>
   </si>
   <si>
-    <t>Amount</t>
-  </si>
-  <si>
-    <t>Alice</t>
-  </si>
-  <si>
-    <t>001234567890</t>
-  </si>
-  <si>
-    <t>021000021</t>
-  </si>
-  <si>
-    <t>1234.00</t>
-  </si>
-  <si>
-    <t>Bob</t>
-  </si>
-  <si>
-    <t>000045678901</t>
-  </si>
-  <si>
-    <t>026009593</t>
-  </si>
-  <si>
-    <t>9999999999999999.99</t>
-  </si>
-  <si>
-    <t>Carol</t>
+    <t>Amount (BDT)</t>
+  </si>
+  <si>
+    <t>Credit Narration</t>
+  </si>
+  <si>
+    <t>Cycle Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SI Start Date
+(DD/MM/YYYY)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SI End Date
+(DD/MM/YYYY)</t>
+  </si>
+  <si>
+    <t>Receiver's Email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Receiver's
+Mobile Number</t>
+  </si>
+  <si>
+    <t>123456789-1</t>
+  </si>
+  <si>
+    <t>John Doe</t>
+  </si>
+  <si>
+    <t>1234567890123</t>
   </si>
   <si>
     <t>123456789</t>
   </si>
   <si>
-    <t>111000025</t>
-  </si>
-  <si>
-    <t>45.67</t>
+    <t>5000.00</t>
+  </si>
+  <si>
+    <t>Instant</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>john.doe@example.com</t>
+  </si>
+  <si>
+    <t>987654321-1</t>
+  </si>
+  <si>
+    <t>Jane Smith</t>
+  </si>
+  <si>
+    <t>9876543210987</t>
+  </si>
+  <si>
+    <t>987654321</t>
+  </si>
+  <si>
+    <t>7500.00</t>
+  </si>
+  <si>
+    <t>jane.smith@example.com</t>
+  </si>
+  <si>
+    <t>456789123-1</t>
+  </si>
+  <si>
+    <t>Bob Johnson</t>
+  </si>
+  <si>
+    <t>4567891234567</t>
+  </si>
+  <si>
+    <t>456789123</t>
+  </si>
+  <si>
+    <t>2000.00</t>
+  </si>
+  <si>
+    <t>bob.johnson@example.com</t>
+  </si>
+  <si>
+    <t>789123456-1</t>
+  </si>
+  <si>
+    <t>Alice Brown</t>
+  </si>
+  <si>
+    <t>7891234567890</t>
+  </si>
+  <si>
+    <t>789123456</t>
+  </si>
+  <si>
+    <t>12000.00</t>
+  </si>
+  <si>
+    <t>Monthly</t>
+  </si>
+  <si>
+    <t>01/01/2025</t>
+  </si>
+  <si>
+    <t>31/12/2025</t>
+  </si>
+  <si>
+    <t>alice.brown@example.com</t>
+  </si>
+  <si>
+    <t>321654987-1</t>
+  </si>
+  <si>
+    <t>Charlie Wilson</t>
+  </si>
+  <si>
+    <t>3216549876543</t>
+  </si>
+  <si>
+    <t>321654987</t>
+  </si>
+  <si>
+    <t>30000.00</t>
+  </si>
+  <si>
+    <t>15/06/2025</t>
+  </si>
+  <si>
+    <t>15/06/2027</t>
+  </si>
+  <si>
+    <t>charlie.wilson@example.com</t>
+  </si>
+  <si>
+    <t>654987321-1</t>
+  </si>
+  <si>
+    <t>Diana Lee</t>
+  </si>
+  <si>
+    <t>6549873210987</t>
+  </si>
+  <si>
+    <t>654987321</t>
+  </si>
+  <si>
+    <t>800.00</t>
+  </si>
+  <si>
+    <t>01/03/2025</t>
+  </si>
+  <si>
+    <t>01/03/2030</t>
+  </si>
+  <si>
+    <t>diana.lee@example.com</t>
   </si>
 </sst>
 </file>
@@ -432,16 +555,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:K7"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="22" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="1" max="11" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -454,47 +574,236 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>7</v>
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>13</v>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>15</v>
+        <v>28</v>
+      </c>
+      <c r="E4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" t="s">
+        <v>39</v>
+      </c>
+      <c r="K5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J6" t="s">
+        <v>47</v>
+      </c>
+      <c r="K6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="J7" t="s">
+        <v>55</v>
+      </c>
+      <c r="K7" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add column 'K' to text formatting in Excel export
</commit_message>
<xml_diff>
--- a/Excel File Generator/Output.xlsx
+++ b/Excel File Generator/Output.xlsx
@@ -627,7 +627,7 @@
       <c r="J2" t="s">
         <v>18</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="2" t="s">
         <v>17</v>
       </c>
     </row>
@@ -662,7 +662,7 @@
       <c r="J3" t="s">
         <v>24</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="2" t="s">
         <v>17</v>
       </c>
     </row>
@@ -697,7 +697,7 @@
       <c r="J4" t="s">
         <v>30</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="2" t="s">
         <v>17</v>
       </c>
     </row>
@@ -732,7 +732,7 @@
       <c r="J5" t="s">
         <v>39</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" s="2" t="s">
         <v>17</v>
       </c>
     </row>
@@ -767,7 +767,7 @@
       <c r="J6" t="s">
         <v>47</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" s="2" t="s">
         <v>17</v>
       </c>
     </row>
@@ -802,7 +802,7 @@
       <c r="J7" t="s">
         <v>55</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" s="2" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>